<commit_message>
Added wait time|additional optimization|Added Test Plan
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/RSTK-9526-SYDATA-Create Extract component transaction.xlsx
+++ b/templates/AutomationOrg/RSTK-9526-SYDATA-Create Extract component transaction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\QA-Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\EventDemo\Parallel-Execution\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A584CD-34FB-4A97-8A86-FF99955857E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54EB0AC-4993-4160-88B4-0759EB62F290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77C97FEF-7E82-40F3-B240-8FA62379481A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Background Processing</t>
   </si>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146DD3D7-6B9F-488C-B01E-10184532587E}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+      <selection activeCell="E3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,20 +485,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>